<commit_message>
added nl-core-careplan profile and mapping + adjusted mappings for NursingIntervention and OutcomeOfCare.
</commit_message>
<xml_diff>
--- a/Mappings/NursingIntervention - STU3.xlsx
+++ b/Mappings/NursingIntervention - STU3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\nicitz-stu3-zibs2017\Profiles-Staging\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\nictiz-stu3-zib2017\Mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,17 +15,12 @@
     <sheet name="NursingIntervention 2017" sheetId="1" r:id="rId1"/>
     <sheet name="Valuesets 2017" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterate="1"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="132">
   <si>
     <t>Concept</t>
   </si>
@@ -392,13 +387,43 @@
   </si>
   <si>
     <t>Procedure.extension:Instruction</t>
+  </si>
+  <si>
+    <t>Careplan</t>
+  </si>
+  <si>
+    <t>.activity.detail.code</t>
+  </si>
+  <si>
+    <t>.activity.detail.reasonReference</t>
+  </si>
+  <si>
+    <t>.activity.detail.performer</t>
+  </si>
+  <si>
+    <t>.activity.detail.scheduledTiming</t>
+  </si>
+  <si>
+    <t>.goal or .activity.detail.goal</t>
+  </si>
+  <si>
+    <t>.activity.detail.extension::MedicalDevice</t>
+  </si>
+  <si>
+    <t>.activity.detail.description</t>
+  </si>
+  <si>
+    <t>Careplan.activity.reference target --&gt; procedureRequest</t>
+  </si>
+  <si>
+    <t>.note</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -439,6 +464,10 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="7">
@@ -551,11 +580,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -632,10 +662,20 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -981,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:R19"/>
+  <dimension ref="B2:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -996,15 +1036,15 @@
     <col min="9" max="10" width="5" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="75" customWidth="1"/>
+    <col min="13" max="13" width="40.5703125" customWidth="1"/>
     <col min="14" max="14" width="20" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="30" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="32.42578125" customWidth="1"/>
-    <col min="17" max="17" width="31.140625" customWidth="1"/>
-    <col min="18" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="17" max="18" width="31.140625" customWidth="1"/>
+    <col min="19" max="1017" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1043,8 +1083,9 @@
       <c r="Q2" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="2:18" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="R2" s="26"/>
+    </row>
+    <row r="3" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="s">
         <v>11</v>
       </c>
@@ -1073,8 +1114,11 @@
         <v>16</v>
       </c>
       <c r="Q3" s="9"/>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="R3" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="10"/>
       <c r="C4" s="11" t="s">
         <v>17</v>
@@ -1111,8 +1155,11 @@
       <c r="Q4" s="24" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="R4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B5" s="10"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
@@ -1132,7 +1179,7 @@
       <c r="P5" s="23"/>
       <c r="Q5" s="24"/>
     </row>
-    <row r="6" spans="2:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B6" s="10"/>
       <c r="C6" s="11" t="s">
         <v>28</v>
@@ -1165,8 +1212,11 @@
         <v>35</v>
       </c>
       <c r="Q6" s="9"/>
-    </row>
-    <row r="7" spans="2:18" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="R6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B7" s="10"/>
       <c r="C7" s="11" t="s">
         <v>36</v>
@@ -1199,8 +1249,11 @@
         <v>41</v>
       </c>
       <c r="Q7" s="9"/>
-    </row>
-    <row r="8" spans="2:18" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="R7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B8" s="10"/>
       <c r="C8" s="11" t="s">
         <v>42</v>
@@ -1232,8 +1285,11 @@
         <v>119</v>
       </c>
       <c r="Q8" s="9"/>
-    </row>
-    <row r="9" spans="2:18" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="R8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B9" s="10"/>
       <c r="C9" s="11" t="s">
         <v>47</v>
@@ -1266,9 +1322,12 @@
         <v>120</v>
       </c>
       <c r="Q9" s="9"/>
-      <c r="R9" s="15"/>
-    </row>
-    <row r="10" spans="2:18" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="R9" t="s">
+        <v>126</v>
+      </c>
+      <c r="S9" s="15"/>
+    </row>
+    <row r="10" spans="2:19" ht="51" x14ac:dyDescent="0.2">
       <c r="B10" s="10"/>
       <c r="C10" s="11" t="s">
         <v>51</v>
@@ -1301,8 +1360,11 @@
         <v>56</v>
       </c>
       <c r="Q10" s="9"/>
-    </row>
-    <row r="11" spans="2:18" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="R10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B11" s="10"/>
       <c r="C11" s="11" t="s">
         <v>57</v>
@@ -1335,8 +1397,11 @@
         <v>61</v>
       </c>
       <c r="Q11" s="9"/>
-    </row>
-    <row r="12" spans="2:18" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="R11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B12" s="10"/>
       <c r="C12" s="11" t="s">
         <v>62</v>
@@ -1369,9 +1434,12 @@
         <v>68</v>
       </c>
       <c r="Q12" s="9"/>
-      <c r="R12" s="15"/>
-    </row>
-    <row r="13" spans="2:18" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="R12" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="S12" s="15"/>
+    </row>
+    <row r="13" spans="2:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="10"/>
       <c r="C13" s="11" t="s">
         <v>69</v>
@@ -1404,9 +1472,12 @@
         <v>121</v>
       </c>
       <c r="Q13" s="9"/>
-      <c r="R13" s="15"/>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="R13" t="s">
+        <v>129</v>
+      </c>
+      <c r="S13" s="15"/>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B14" s="16"/>
       <c r="C14" s="17" t="s">
         <v>74</v>
@@ -1437,8 +1508,11 @@
         <v>79</v>
       </c>
       <c r="Q14" s="9"/>
-    </row>
-    <row r="15" spans="2:18" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="R14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B15" s="10"/>
       <c r="C15" s="21"/>
       <c r="D15" s="21" t="s">
@@ -1471,8 +1545,11 @@
         <v>86</v>
       </c>
       <c r="Q15" s="9"/>
-    </row>
-    <row r="16" spans="2:18" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="R15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B16" s="10"/>
       <c r="C16" s="21"/>
       <c r="D16" s="21" t="s">
@@ -1505,9 +1582,12 @@
         <v>86</v>
       </c>
       <c r="Q16" s="9"/>
-      <c r="R16" s="15"/>
-    </row>
-    <row r="17" spans="2:17" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="R16" t="s">
+        <v>125</v>
+      </c>
+      <c r="S16" s="15"/>
+    </row>
+    <row r="17" spans="2:18" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B17" s="10"/>
       <c r="C17" s="21"/>
       <c r="D17" s="21" t="s">
@@ -1540,8 +1620,11 @@
         <v>86</v>
       </c>
       <c r="Q17" s="9"/>
-    </row>
-    <row r="18" spans="2:17" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="R17" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B18" s="10"/>
       <c r="C18" s="21" t="s">
         <v>97</v>
@@ -1574,8 +1657,11 @@
         <v>101</v>
       </c>
       <c r="Q18" s="9"/>
-    </row>
-    <row r="19" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="R18" s="28" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B19" s="10"/>
       <c r="C19" s="21" t="s">
         <v>102</v>
@@ -1610,6 +1696,9 @@
         <v>107</v>
       </c>
       <c r="Q19" s="9"/>
+      <c r="R19" s="28" t="s">
+        <v>131</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1633,6 +1722,17 @@
     <hyperlink ref="O16" r:id="rId5"/>
     <hyperlink ref="O17" r:id="rId6"/>
     <hyperlink ref="O18" r:id="rId7"/>
+    <hyperlink ref="Z3" r:id="rId8" display="SNOMED CT: 9632001 Nursing procedure"/>
+    <hyperlink ref="AA4" location="InterventionNICCodelist!A1" display="InterventionNICCodelist"/>
+    <hyperlink ref="AA5" location="InterventionSnomedCodelist!A1" display="InterventionSnomedCodelist"/>
+    <hyperlink ref="AA6" r:id="rId9" display="This is a reference to the rootconcept of information model Problem."/>
+    <hyperlink ref="AA7" r:id="rId10" display="This is a reference to the rootconcept of information model TreatmentObjective."/>
+    <hyperlink ref="AA12" r:id="rId11" display="This is a reference to the rootconcept of information model  MedicalDevice."/>
+    <hyperlink ref="AA15" r:id="rId12" display="This is a reference to the rootconcept of information model HealthProfessional."/>
+    <hyperlink ref="AA16" r:id="rId13" display="This is a reference to the rootconcept of information model ContactPerson."/>
+    <hyperlink ref="AA17" r:id="rId14" display="This is a reference to the rootconcept of information model Patient."/>
+    <hyperlink ref="AA18" r:id="rId15" display="This is a reference to the rootconcept of information model HealthProfessional."/>
+    <hyperlink ref="Z19" r:id="rId16" display="LOINC: 48767-8 Annotation comment [Interpretation] Narrative"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
manually merged changes in develop branch of BgLZ related artefactes for public consultation
</commit_message>
<xml_diff>
--- a/Mappings/NursingIntervention - STU3.xlsx
+++ b/Mappings/NursingIntervention - STU3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\nicitz-stu3-zibs2017\Profiles-Staging\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\nictiz-stu3-zib2017\Mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,17 +15,12 @@
     <sheet name="NursingIntervention 2017" sheetId="1" r:id="rId1"/>
     <sheet name="Valuesets 2017" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterate="1"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="132">
   <si>
     <t>Concept</t>
   </si>
@@ -392,13 +387,43 @@
   </si>
   <si>
     <t>Procedure.extension:Instruction</t>
+  </si>
+  <si>
+    <t>Careplan</t>
+  </si>
+  <si>
+    <t>.activity.detail.code</t>
+  </si>
+  <si>
+    <t>.activity.detail.reasonReference</t>
+  </si>
+  <si>
+    <t>.activity.detail.performer</t>
+  </si>
+  <si>
+    <t>.activity.detail.scheduledTiming</t>
+  </si>
+  <si>
+    <t>.goal or .activity.detail.goal</t>
+  </si>
+  <si>
+    <t>.activity.detail.extension::MedicalDevice</t>
+  </si>
+  <si>
+    <t>.activity.detail.description</t>
+  </si>
+  <si>
+    <t>Careplan.activity.reference target --&gt; procedureRequest</t>
+  </si>
+  <si>
+    <t>.note</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -439,6 +464,10 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="7">
@@ -551,11 +580,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -632,10 +662,20 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -981,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:R19"/>
+  <dimension ref="B2:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -996,15 +1036,15 @@
     <col min="9" max="10" width="5" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="75" customWidth="1"/>
+    <col min="13" max="13" width="40.5703125" customWidth="1"/>
     <col min="14" max="14" width="20" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="30" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="32.42578125" customWidth="1"/>
-    <col min="17" max="17" width="31.140625" customWidth="1"/>
-    <col min="18" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="17" max="18" width="31.140625" customWidth="1"/>
+    <col min="19" max="1017" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1043,8 +1083,9 @@
       <c r="Q2" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="2:18" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="R2" s="26"/>
+    </row>
+    <row r="3" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="s">
         <v>11</v>
       </c>
@@ -1073,8 +1114,11 @@
         <v>16</v>
       </c>
       <c r="Q3" s="9"/>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="R3" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="10"/>
       <c r="C4" s="11" t="s">
         <v>17</v>
@@ -1111,8 +1155,11 @@
       <c r="Q4" s="24" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="R4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B5" s="10"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
@@ -1132,7 +1179,7 @@
       <c r="P5" s="23"/>
       <c r="Q5" s="24"/>
     </row>
-    <row r="6" spans="2:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B6" s="10"/>
       <c r="C6" s="11" t="s">
         <v>28</v>
@@ -1165,8 +1212,11 @@
         <v>35</v>
       </c>
       <c r="Q6" s="9"/>
-    </row>
-    <row r="7" spans="2:18" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="R6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B7" s="10"/>
       <c r="C7" s="11" t="s">
         <v>36</v>
@@ -1199,8 +1249,11 @@
         <v>41</v>
       </c>
       <c r="Q7" s="9"/>
-    </row>
-    <row r="8" spans="2:18" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="R7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B8" s="10"/>
       <c r="C8" s="11" t="s">
         <v>42</v>
@@ -1232,8 +1285,11 @@
         <v>119</v>
       </c>
       <c r="Q8" s="9"/>
-    </row>
-    <row r="9" spans="2:18" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="R8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B9" s="10"/>
       <c r="C9" s="11" t="s">
         <v>47</v>
@@ -1266,9 +1322,12 @@
         <v>120</v>
       </c>
       <c r="Q9" s="9"/>
-      <c r="R9" s="15"/>
-    </row>
-    <row r="10" spans="2:18" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="R9" t="s">
+        <v>126</v>
+      </c>
+      <c r="S9" s="15"/>
+    </row>
+    <row r="10" spans="2:19" ht="51" x14ac:dyDescent="0.2">
       <c r="B10" s="10"/>
       <c r="C10" s="11" t="s">
         <v>51</v>
@@ -1301,8 +1360,11 @@
         <v>56</v>
       </c>
       <c r="Q10" s="9"/>
-    </row>
-    <row r="11" spans="2:18" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="R10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B11" s="10"/>
       <c r="C11" s="11" t="s">
         <v>57</v>
@@ -1335,8 +1397,11 @@
         <v>61</v>
       </c>
       <c r="Q11" s="9"/>
-    </row>
-    <row r="12" spans="2:18" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="R11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B12" s="10"/>
       <c r="C12" s="11" t="s">
         <v>62</v>
@@ -1369,9 +1434,12 @@
         <v>68</v>
       </c>
       <c r="Q12" s="9"/>
-      <c r="R12" s="15"/>
-    </row>
-    <row r="13" spans="2:18" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="R12" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="S12" s="15"/>
+    </row>
+    <row r="13" spans="2:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="10"/>
       <c r="C13" s="11" t="s">
         <v>69</v>
@@ -1404,9 +1472,12 @@
         <v>121</v>
       </c>
       <c r="Q13" s="9"/>
-      <c r="R13" s="15"/>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="R13" t="s">
+        <v>129</v>
+      </c>
+      <c r="S13" s="15"/>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B14" s="16"/>
       <c r="C14" s="17" t="s">
         <v>74</v>
@@ -1437,8 +1508,11 @@
         <v>79</v>
       </c>
       <c r="Q14" s="9"/>
-    </row>
-    <row r="15" spans="2:18" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="R14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B15" s="10"/>
       <c r="C15" s="21"/>
       <c r="D15" s="21" t="s">
@@ -1471,8 +1545,11 @@
         <v>86</v>
       </c>
       <c r="Q15" s="9"/>
-    </row>
-    <row r="16" spans="2:18" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="R15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B16" s="10"/>
       <c r="C16" s="21"/>
       <c r="D16" s="21" t="s">
@@ -1505,9 +1582,12 @@
         <v>86</v>
       </c>
       <c r="Q16" s="9"/>
-      <c r="R16" s="15"/>
-    </row>
-    <row r="17" spans="2:17" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="R16" t="s">
+        <v>125</v>
+      </c>
+      <c r="S16" s="15"/>
+    </row>
+    <row r="17" spans="2:18" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B17" s="10"/>
       <c r="C17" s="21"/>
       <c r="D17" s="21" t="s">
@@ -1540,8 +1620,11 @@
         <v>86</v>
       </c>
       <c r="Q17" s="9"/>
-    </row>
-    <row r="18" spans="2:17" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="R17" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B18" s="10"/>
       <c r="C18" s="21" t="s">
         <v>97</v>
@@ -1574,8 +1657,11 @@
         <v>101</v>
       </c>
       <c r="Q18" s="9"/>
-    </row>
-    <row r="19" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="R18" s="28" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B19" s="10"/>
       <c r="C19" s="21" t="s">
         <v>102</v>
@@ -1610,6 +1696,9 @@
         <v>107</v>
       </c>
       <c r="Q19" s="9"/>
+      <c r="R19" s="28" t="s">
+        <v>131</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1633,6 +1722,17 @@
     <hyperlink ref="O16" r:id="rId5"/>
     <hyperlink ref="O17" r:id="rId6"/>
     <hyperlink ref="O18" r:id="rId7"/>
+    <hyperlink ref="Z3" r:id="rId8" display="SNOMED CT: 9632001 Nursing procedure"/>
+    <hyperlink ref="AA4" location="InterventionNICCodelist!A1" display="InterventionNICCodelist"/>
+    <hyperlink ref="AA5" location="InterventionSnomedCodelist!A1" display="InterventionSnomedCodelist"/>
+    <hyperlink ref="AA6" r:id="rId9" display="This is a reference to the rootconcept of information model Problem."/>
+    <hyperlink ref="AA7" r:id="rId10" display="This is a reference to the rootconcept of information model TreatmentObjective."/>
+    <hyperlink ref="AA12" r:id="rId11" display="This is a reference to the rootconcept of information model  MedicalDevice."/>
+    <hyperlink ref="AA15" r:id="rId12" display="This is a reference to the rootconcept of information model HealthProfessional."/>
+    <hyperlink ref="AA16" r:id="rId13" display="This is a reference to the rootconcept of information model ContactPerson."/>
+    <hyperlink ref="AA17" r:id="rId14" display="This is a reference to the rootconcept of information model Patient."/>
+    <hyperlink ref="AA18" r:id="rId15" display="This is a reference to the rootconcept of information model HealthProfessional."/>
+    <hyperlink ref="Z19" r:id="rId16" display="LOINC: 48767-8 Annotation comment [Interpretation] Narrative"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>